<commit_message>
Korrektur der NaiS-Einheiten AR
</commit_message>
<xml_diff>
--- a/AR_nais_einheiten_unique_mf.xlsx
+++ b/AR_nais_einheiten_unique_mf.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frehnerm\Documents\excel\Aufträge\Sensi CH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\develops\sensitivewaldstandorteCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A9C2F7-73DB-4F33-A8EE-67C2432858D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1E04B5-C272-4EE3-BAA4-A8B7EBBC31B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29085" yWindow="-5400" windowWidth="25530" windowHeight="20250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="13944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="458">
   <si>
     <t>DTWGEINHEI</t>
   </si>
@@ -1297,9 +1297,6 @@
     <t>12S(29)</t>
   </si>
   <si>
-    <t>12w(12Fe)</t>
-  </si>
-  <si>
     <t>13h(20)</t>
   </si>
   <si>
@@ -1385,6 +1382,18 @@
   </si>
   <si>
     <t>Achtung, neue Einheit, neuer Projektionsweg notwendig</t>
+  </si>
+  <si>
+    <t>18v(53Ta)</t>
+  </si>
+  <si>
+    <t>22(12a)</t>
+  </si>
+  <si>
+    <t>26(12a)</t>
+  </si>
+  <si>
+    <t>12w(12aFe)</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1465,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1772,23 +1781,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="D93" workbookViewId="0">
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.1015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1015625" customWidth="1"/>
+    <col min="8" max="8" width="11.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>408</v>
       </c>
@@ -1820,7 +1829,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>388</v>
       </c>
@@ -1866,7 +1875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>390</v>
       </c>
@@ -1892,7 +1901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>400</v>
       </c>
@@ -1918,7 +1927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>422</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>1124</v>
       </c>
@@ -1970,7 +1979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>1206</v>
       </c>
@@ -1996,7 +2005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>1338</v>
       </c>
@@ -2022,7 +2031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>1349</v>
       </c>
@@ -2048,7 +2057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>1777</v>
       </c>
@@ -2074,7 +2083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>1782</v>
       </c>
@@ -2100,7 +2109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>2356</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>2361</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>2381</v>
       </c>
@@ -2178,7 +2187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>2398</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>2399</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>2411</v>
       </c>
@@ -2250,7 +2259,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>2428</v>
       </c>
@@ -2276,7 +2285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>2564</v>
       </c>
@@ -2302,7 +2311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>2587</v>
       </c>
@@ -2328,7 +2337,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>2789</v>
       </c>
@@ -2354,7 +2363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>2922</v>
       </c>
@@ -2380,7 +2389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>4014</v>
       </c>
@@ -2406,7 +2415,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>4015</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>4028</v>
       </c>
@@ -2458,7 +2467,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>4090</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>4494</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>4996</v>
       </c>
@@ -2536,7 +2545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>4999</v>
       </c>
@@ -2556,7 +2565,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>5000</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>5006</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>5080</v>
       </c>
@@ -2634,7 +2643,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>7596</v>
       </c>
@@ -2660,7 +2669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>7597</v>
       </c>
@@ -2686,7 +2695,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>7600</v>
       </c>
@@ -2712,7 +2721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>8755</v>
       </c>
@@ -2738,7 +2747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>8923</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>8924</v>
       </c>
@@ -2790,7 +2799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>8935</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>9524</v>
       </c>
@@ -2842,7 +2851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>9528</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>9532</v>
       </c>
@@ -2894,7 +2903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>9534</v>
       </c>
@@ -2920,7 +2929,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>9556</v>
       </c>
@@ -2946,7 +2955,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>9557</v>
       </c>
@@ -2972,7 +2981,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>9566</v>
       </c>
@@ -2998,7 +3007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>10161</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>10180</v>
       </c>
@@ -3050,7 +3059,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>10484</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>10488</v>
       </c>
@@ -3102,7 +3111,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>10491</v>
       </c>
@@ -3128,10 +3137,10 @@
         <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>10547</v>
       </c>
@@ -3157,10 +3166,10 @@
         <v>33</v>
       </c>
       <c r="J53" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>10729</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>11011</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>11013</v>
       </c>
@@ -3238,7 +3247,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>11015</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>11073</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>11078</v>
       </c>
@@ -3316,7 +3325,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>11081</v>
       </c>
@@ -3342,7 +3351,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>11086</v>
       </c>
@@ -3368,7 +3377,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>11087</v>
       </c>
@@ -3394,7 +3403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>11094</v>
       </c>
@@ -3420,7 +3429,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>11322</v>
       </c>
@@ -3446,7 +3455,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>11350</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>11620</v>
       </c>
@@ -3498,7 +3507,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>11621</v>
       </c>
@@ -3524,7 +3533,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>11625</v>
       </c>
@@ -3553,7 +3562,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>11625</v>
       </c>
@@ -3573,7 +3582,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>11632</v>
       </c>
@@ -3599,7 +3608,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>11667</v>
       </c>
@@ -3628,7 +3637,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>11667</v>
       </c>
@@ -3648,7 +3657,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>11674</v>
       </c>
@@ -3674,7 +3683,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>11676</v>
       </c>
@@ -3700,7 +3709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>11680</v>
       </c>
@@ -3726,7 +3735,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>11681</v>
       </c>
@@ -3752,7 +3761,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>11686</v>
       </c>
@@ -3778,7 +3787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>11772</v>
       </c>
@@ -3804,7 +3813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>11807</v>
       </c>
@@ -3830,7 +3839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>11812</v>
       </c>
@@ -3856,7 +3865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>11845</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>11863</v>
       </c>
@@ -3908,7 +3917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>11876</v>
       </c>
@@ -3934,7 +3943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>11881</v>
       </c>
@@ -3960,7 +3969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>11882</v>
       </c>
@@ -3986,7 +3995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>11891</v>
       </c>
@@ -4012,7 +4021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>13016</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>13017</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>13021</v>
       </c>
@@ -4078,7 +4087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>14185</v>
       </c>
@@ -4104,7 +4113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>14320</v>
       </c>
@@ -4130,7 +4139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>14522</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>14569</v>
       </c>
@@ -4182,7 +4191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>15413</v>
       </c>
@@ -4208,7 +4217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>15414</v>
       </c>
@@ -4234,7 +4243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>15420</v>
       </c>
@@ -4260,7 +4269,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>15421</v>
       </c>
@@ -4286,7 +4295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>15425</v>
       </c>
@@ -4312,7 +4321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>15532</v>
       </c>
@@ -4338,7 +4347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>15548</v>
       </c>
@@ -4358,7 +4367,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>15549</v>
       </c>
@@ -4378,7 +4387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>15550</v>
       </c>
@@ -4398,7 +4407,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>15551</v>
       </c>
@@ -4418,7 +4427,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>15552</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>15553</v>
       </c>
@@ -4458,7 +4467,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>15554</v>
       </c>
@@ -4478,7 +4487,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>15555</v>
       </c>
@@ -4498,7 +4507,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>15557</v>
       </c>
@@ -4518,7 +4527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>15558</v>
       </c>
@@ -4532,13 +4541,13 @@
         <v>20</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c r="I109" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>15560</v>
       </c>
@@ -4558,7 +4567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>15570</v>
       </c>
@@ -4578,7 +4587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>15572</v>
       </c>
@@ -4598,7 +4607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>15573</v>
       </c>
@@ -4618,7 +4627,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>15574</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>15579</v>
       </c>
@@ -4658,7 +4667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>15583</v>
       </c>
@@ -4672,13 +4681,13 @@
         <v>35</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I116" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>15585</v>
       </c>
@@ -4692,13 +4701,13 @@
         <v>9</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I117" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>15586</v>
       </c>
@@ -4718,7 +4727,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>15587</v>
       </c>
@@ -4738,7 +4747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>15589</v>
       </c>
@@ -4758,7 +4767,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>15592</v>
       </c>
@@ -4772,13 +4781,13 @@
         <v>44</v>
       </c>
       <c r="H121" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I121" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>15593</v>
       </c>
@@ -4792,13 +4801,13 @@
         <v>44</v>
       </c>
       <c r="H122" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I122" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>15595</v>
       </c>
@@ -4812,13 +4821,13 @@
         <v>44</v>
       </c>
       <c r="H123" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I123" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>15598</v>
       </c>
@@ -4838,7 +4847,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1">
         <v>15600</v>
       </c>
@@ -4858,7 +4867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>15610</v>
       </c>
@@ -4878,7 +4887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>15613</v>
       </c>
@@ -4898,7 +4907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>15628</v>
       </c>
@@ -4918,7 +4927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>15630</v>
       </c>
@@ -4938,7 +4947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>15634</v>
       </c>
@@ -4958,7 +4967,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>15636</v>
       </c>
@@ -4979,7 +4988,7 @@
       </c>
       <c r="N131" s="4"/>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1">
         <v>15660</v>
       </c>
@@ -4999,7 +5008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>15661</v>
       </c>
@@ -5019,7 +5028,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1">
         <v>15665</v>
       </c>
@@ -5033,13 +5042,13 @@
         <v>53</v>
       </c>
       <c r="H134" s="4" t="s">
-        <v>208</v>
+        <v>454</v>
       </c>
       <c r="I134" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>15666</v>
       </c>
@@ -5053,13 +5062,13 @@
         <v>53</v>
       </c>
       <c r="H135" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I135" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>15672</v>
       </c>
@@ -5079,7 +5088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>15702</v>
       </c>
@@ -5099,7 +5108,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>15703</v>
       </c>
@@ -5119,7 +5128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>15707</v>
       </c>
@@ -5139,7 +5148,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>15722</v>
       </c>
@@ -5159,7 +5168,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>15728</v>
       </c>
@@ -5176,10 +5185,10 @@
         <v>215</v>
       </c>
       <c r="I141" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>15729</v>
       </c>
@@ -5199,7 +5208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>15739</v>
       </c>
@@ -5219,7 +5228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>15744</v>
       </c>
@@ -5236,10 +5245,10 @@
         <v>218</v>
       </c>
       <c r="I144" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>15745</v>
       </c>
@@ -5259,7 +5268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>15746</v>
       </c>
@@ -5279,7 +5288,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>15748</v>
       </c>
@@ -5299,7 +5308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1">
         <v>15778</v>
       </c>
@@ -5319,7 +5328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>15779</v>
       </c>
@@ -5339,7 +5348,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>15780</v>
       </c>
@@ -5359,7 +5368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1">
         <v>15810</v>
       </c>
@@ -5379,7 +5388,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>15850</v>
       </c>
@@ -5399,7 +5408,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>15859</v>
       </c>
@@ -5419,7 +5428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>15865</v>
       </c>
@@ -5439,7 +5448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>15866</v>
       </c>
@@ -5459,7 +5468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>15868</v>
       </c>
@@ -5479,7 +5488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>15877</v>
       </c>
@@ -5499,7 +5508,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>15879</v>
       </c>
@@ -5519,7 +5528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>15880</v>
       </c>
@@ -5539,7 +5548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>15881</v>
       </c>
@@ -5559,7 +5568,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>15882</v>
       </c>
@@ -5579,7 +5588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>15887</v>
       </c>
@@ -5599,7 +5608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>15890</v>
       </c>
@@ -5616,10 +5625,10 @@
         <v>237</v>
       </c>
       <c r="I163" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>15891</v>
       </c>
@@ -5639,7 +5648,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>15892</v>
       </c>
@@ -5659,7 +5668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>15916</v>
       </c>
@@ -5679,7 +5688,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>15980</v>
       </c>
@@ -5699,7 +5708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>15986</v>
       </c>
@@ -5719,7 +5728,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>15999</v>
       </c>
@@ -5739,7 +5748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>16056</v>
       </c>
@@ -5759,7 +5768,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>16066</v>
       </c>
@@ -5779,7 +5788,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>16067</v>
       </c>
@@ -5799,7 +5808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>16415</v>
       </c>
@@ -5819,7 +5828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>16416</v>
       </c>
@@ -5839,7 +5848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1">
         <v>16422</v>
       </c>
@@ -5856,10 +5865,10 @@
         <v>249</v>
       </c>
       <c r="I175" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>16423</v>
       </c>
@@ -5879,7 +5888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>16425</v>
       </c>
@@ -5899,7 +5908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>16426</v>
       </c>
@@ -5919,7 +5928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>16434</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>16438</v>
       </c>
@@ -5959,7 +5968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>16441</v>
       </c>
@@ -5979,7 +5988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>16454</v>
       </c>
@@ -5999,7 +6008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>16456</v>
       </c>
@@ -6019,7 +6028,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>16457</v>
       </c>
@@ -6039,7 +6048,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>16458</v>
       </c>
@@ -6059,7 +6068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>16459</v>
       </c>
@@ -6079,7 +6088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>16478</v>
       </c>
@@ -6099,7 +6108,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>16541</v>
       </c>
@@ -6119,7 +6128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>16543</v>
       </c>
@@ -6139,7 +6148,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>16544</v>
       </c>
@@ -6159,7 +6168,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>16592</v>
       </c>
@@ -6179,7 +6188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1">
         <v>16602</v>
       </c>
@@ -6199,7 +6208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1">
         <v>16603</v>
       </c>
@@ -6219,7 +6228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="1">
         <v>16604</v>
       </c>
@@ -6239,7 +6248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="1">
         <v>16615</v>
       </c>
@@ -6259,7 +6268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" s="1">
         <v>16619</v>
       </c>
@@ -6279,7 +6288,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" s="1">
         <v>16620</v>
       </c>
@@ -6299,7 +6308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="1">
         <v>16639</v>
       </c>
@@ -6319,7 +6328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" s="1">
         <v>16649</v>
       </c>
@@ -6336,10 +6345,10 @@
         <v>273</v>
       </c>
       <c r="I199" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" s="1">
         <v>16650</v>
       </c>
@@ -6359,7 +6368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" s="1">
         <v>16653</v>
       </c>
@@ -6379,7 +6388,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" s="1">
         <v>16655</v>
       </c>
@@ -6399,7 +6408,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" s="1">
         <v>16667</v>
       </c>
@@ -6419,7 +6428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" s="1">
         <v>16669</v>
       </c>
@@ -6439,7 +6448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" s="1">
         <v>16670</v>
       </c>
@@ -6459,7 +6468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" s="1">
         <v>16671</v>
       </c>
@@ -6479,7 +6488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="1">
         <v>16672</v>
       </c>
@@ -6499,7 +6508,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="1">
         <v>16683</v>
       </c>
@@ -6519,7 +6528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="1">
         <v>16709</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="1">
         <v>16742</v>
       </c>
@@ -6559,7 +6568,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" s="1">
         <v>16757</v>
       </c>
@@ -6579,7 +6588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="1">
         <v>16760</v>
       </c>
@@ -6599,7 +6608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="1">
         <v>16771</v>
       </c>
@@ -6619,7 +6628,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="1">
         <v>16789</v>
       </c>
@@ -6639,7 +6648,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="1">
         <v>16794</v>
       </c>
@@ -6659,7 +6668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="1">
         <v>16808</v>
       </c>
@@ -6673,13 +6682,13 @@
         <v>75</v>
       </c>
       <c r="H216" s="4" t="s">
-        <v>290</v>
+        <v>455</v>
       </c>
       <c r="I216" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="1">
         <v>16809</v>
       </c>
@@ -6699,7 +6708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="1">
         <v>16810</v>
       </c>
@@ -6713,13 +6722,13 @@
         <v>80</v>
       </c>
       <c r="H218" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I218" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="1">
         <v>16812</v>
       </c>
@@ -6727,13 +6736,13 @@
         <v>293</v>
       </c>
       <c r="H219" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I219" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="1">
         <v>16813</v>
       </c>
@@ -6753,7 +6762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="1">
         <v>16819</v>
       </c>
@@ -6773,7 +6782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="1">
         <v>16853</v>
       </c>
@@ -6793,7 +6802,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="1">
         <v>16854</v>
       </c>
@@ -6813,7 +6822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="1">
         <v>16856</v>
       </c>
@@ -6833,7 +6842,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1">
         <v>16857</v>
       </c>
@@ -6847,13 +6856,13 @@
         <v>87</v>
       </c>
       <c r="H225" s="4" t="s">
-        <v>299</v>
+        <v>456</v>
       </c>
       <c r="I225" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1">
         <v>16858</v>
       </c>
@@ -6873,7 +6882,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" s="1">
         <v>16859</v>
       </c>
@@ -6893,7 +6902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="1">
         <v>16860</v>
       </c>
@@ -6919,7 +6928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" s="1">
         <v>16877</v>
       </c>
@@ -6939,7 +6948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" s="1">
         <v>16878</v>
       </c>
@@ -6959,7 +6968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" s="1">
         <v>16881</v>
       </c>
@@ -6979,7 +6988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" s="1">
         <v>16885</v>
       </c>
@@ -6999,7 +7008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" s="1">
         <v>16886</v>
       </c>
@@ -7019,7 +7028,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1">
         <v>16889</v>
       </c>
@@ -7039,7 +7048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1">
         <v>16890</v>
       </c>
@@ -7059,7 +7068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1">
         <v>16900</v>
       </c>
@@ -7079,7 +7088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1">
         <v>16901</v>
       </c>
@@ -7099,7 +7108,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1">
         <v>16919</v>
       </c>
@@ -7119,7 +7128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1">
         <v>16920</v>
       </c>
@@ -7139,7 +7148,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1">
         <v>16934</v>
       </c>
@@ -7159,7 +7168,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1">
         <v>16942</v>
       </c>
@@ -7176,10 +7185,10 @@
         <v>316</v>
       </c>
       <c r="I241" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1">
         <v>16943</v>
       </c>
@@ -7193,13 +7202,13 @@
         <v>101</v>
       </c>
       <c r="H242" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I242" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1">
         <v>16945</v>
       </c>
@@ -7219,7 +7228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1">
         <v>16946</v>
       </c>
@@ -7239,7 +7248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1">
         <v>16947</v>
       </c>
@@ -7259,7 +7268,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1">
         <v>17024</v>
       </c>
@@ -7279,7 +7288,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="1">
         <v>17029</v>
       </c>
@@ -7299,7 +7308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="1">
         <v>17034</v>
       </c>
@@ -7319,7 +7328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="1">
         <v>17037</v>
       </c>
@@ -7339,7 +7348,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="1">
         <v>17065</v>
       </c>
@@ -7359,7 +7368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="1">
         <v>17067</v>
       </c>
@@ -7373,13 +7382,13 @@
         <v>112</v>
       </c>
       <c r="H251" t="s">
+        <v>437</v>
+      </c>
+      <c r="I251" t="s">
         <v>438</v>
       </c>
-      <c r="I251" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1">
         <v>17068</v>
       </c>
@@ -7396,10 +7405,10 @@
         <v>327</v>
       </c>
       <c r="I252" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1">
         <v>17070</v>
       </c>
@@ -7419,7 +7428,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" s="1">
         <v>17074</v>
       </c>
@@ -7439,7 +7448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="1">
         <v>17076</v>
       </c>
@@ -7459,7 +7468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="1">
         <v>17077</v>
       </c>
@@ -7479,7 +7488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1">
         <v>17080</v>
       </c>
@@ -7499,7 +7508,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1">
         <v>17082</v>
       </c>
@@ -7519,7 +7528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1">
         <v>17083</v>
       </c>
@@ -7539,7 +7548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1">
         <v>17084</v>
       </c>
@@ -7559,7 +7568,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1">
         <v>17090</v>
       </c>
@@ -7579,7 +7588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" s="1">
         <v>17095</v>
       </c>
@@ -7599,7 +7608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="1">
         <v>17102</v>
       </c>
@@ -7619,7 +7628,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="1">
         <v>17104</v>
       </c>
@@ -7633,13 +7642,13 @@
         <v>115</v>
       </c>
       <c r="H264" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I264" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="1">
         <v>17105</v>
       </c>
@@ -7656,10 +7665,10 @@
         <v>341</v>
       </c>
       <c r="I265" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="1">
         <v>17106</v>
       </c>
@@ -7679,7 +7688,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1">
         <v>17108</v>
       </c>
@@ -7696,10 +7705,10 @@
         <v>343</v>
       </c>
       <c r="I267" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1">
         <v>17109</v>
       </c>
@@ -7719,7 +7728,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1">
         <v>17111</v>
       </c>
@@ -7739,7 +7748,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" s="1">
         <v>17112</v>
       </c>
@@ -7753,13 +7762,13 @@
         <v>128</v>
       </c>
       <c r="H270" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I270" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="1">
         <v>17113</v>
       </c>
@@ -7779,7 +7788,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" s="1">
         <v>17114</v>
       </c>
@@ -7799,7 +7808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" s="1">
         <v>17115</v>
       </c>
@@ -7819,7 +7828,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="1">
         <v>17116</v>
       </c>
@@ -7839,7 +7848,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" s="1">
         <v>17117</v>
       </c>
@@ -7859,7 +7868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" s="1">
         <v>17128</v>
       </c>
@@ -7879,7 +7888,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1">
         <v>17129</v>
       </c>
@@ -7899,7 +7908,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1">
         <v>17131</v>
       </c>
@@ -7919,7 +7928,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1">
         <v>17132</v>
       </c>
@@ -7939,7 +7948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="1">
         <v>17134</v>
       </c>
@@ -7953,13 +7962,13 @@
         <v>16</v>
       </c>
       <c r="H280" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I280" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1">
         <v>17135</v>
       </c>
@@ -7973,13 +7982,13 @@
         <v>16</v>
       </c>
       <c r="H281" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I281" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1">
         <v>17139</v>
       </c>
@@ -7999,7 +8008,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1">
         <v>17140</v>
       </c>
@@ -8013,7 +8022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1">
         <v>17143</v>
       </c>
@@ -8033,7 +8042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1">
         <v>17144</v>
       </c>
@@ -8053,7 +8062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1">
         <v>17147</v>
       </c>
@@ -8067,13 +8076,13 @@
         <v>22</v>
       </c>
       <c r="H286" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I286" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1">
         <v>17148</v>
       </c>
@@ -8093,7 +8102,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1">
         <v>17149</v>
       </c>
@@ -8107,13 +8116,13 @@
         <v>20</v>
       </c>
       <c r="H288" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I288" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1">
         <v>17150</v>
       </c>
@@ -8133,7 +8142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1">
         <v>17152</v>
       </c>
@@ -8153,7 +8162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1">
         <v>17153</v>
       </c>
@@ -8167,13 +8176,13 @@
         <v>9</v>
       </c>
       <c r="H291" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I291" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1">
         <v>17156</v>
       </c>
@@ -8193,7 +8202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1">
         <v>17162</v>
       </c>
@@ -8207,13 +8216,13 @@
         <v>44</v>
       </c>
       <c r="H293" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I293" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1">
         <v>17164</v>
       </c>
@@ -8227,13 +8236,13 @@
         <v>44</v>
       </c>
       <c r="H294" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I294" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1">
         <v>17166</v>
       </c>
@@ -8253,7 +8262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1">
         <v>17167</v>
       </c>
@@ -8273,7 +8282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1">
         <v>17168</v>
       </c>
@@ -8293,7 +8302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1">
         <v>17169</v>
       </c>
@@ -8313,7 +8322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1">
         <v>17170</v>
       </c>
@@ -8333,7 +8342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" s="1">
         <v>17177</v>
       </c>
@@ -8347,13 +8356,13 @@
         <v>53</v>
       </c>
       <c r="H300" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I300" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" s="1">
         <v>17178</v>
       </c>
@@ -8373,7 +8382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" s="1">
         <v>17179</v>
       </c>
@@ -8393,7 +8402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="1">
         <v>17187</v>
       </c>
@@ -8413,7 +8422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" s="1">
         <v>17188</v>
       </c>
@@ -8433,7 +8442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="1">
         <v>17189</v>
       </c>
@@ -8453,7 +8462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" s="1">
         <v>17190</v>
       </c>
@@ -8473,7 +8482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" s="1">
         <v>17192</v>
       </c>
@@ -8493,7 +8502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" s="1">
         <v>17193</v>
       </c>
@@ -8513,7 +8522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="1">
         <v>17195</v>
       </c>
@@ -8533,7 +8542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" s="1">
         <v>17196</v>
       </c>
@@ -8553,7 +8562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="1">
         <v>17197</v>
       </c>
@@ -8573,7 +8582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" s="1">
         <v>17198</v>
       </c>
@@ -8593,7 +8602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="1">
         <v>17199</v>
       </c>
@@ -8613,7 +8622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="1">
         <v>17200</v>
       </c>
@@ -8627,13 +8636,13 @@
         <v>84</v>
       </c>
       <c r="H314" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I314" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" s="1">
         <v>17207</v>
       </c>
@@ -8647,13 +8656,13 @@
         <v>84</v>
       </c>
       <c r="H315" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I315" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="1">
         <v>17208</v>
       </c>
@@ -8673,7 +8682,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" s="1">
         <v>17210</v>
       </c>
@@ -8693,7 +8702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="1">
         <v>17214</v>
       </c>
@@ -8713,7 +8722,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="1">
         <v>17216</v>
       </c>
@@ -8736,7 +8745,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="1">
         <v>17216</v>
       </c>
@@ -8756,7 +8765,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" s="1">
         <v>17218</v>
       </c>
@@ -8770,13 +8779,13 @@
         <v>122</v>
       </c>
       <c r="H321" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I321" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="1">
         <v>17219</v>
       </c>
@@ -8799,7 +8808,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" s="1">
         <v>17219</v>
       </c>
@@ -8819,7 +8828,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" s="1">
         <v>17220</v>
       </c>
@@ -8839,7 +8848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" s="1">
         <v>17221</v>
       </c>
@@ -8859,7 +8868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="1">
         <v>17222</v>
       </c>
@@ -8873,13 +8882,13 @@
         <v>53</v>
       </c>
       <c r="H326" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I326" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" s="1">
         <v>17223</v>
       </c>
@@ -8899,7 +8908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" s="1">
         <v>17224</v>
       </c>
@@ -8919,7 +8928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="1">
         <v>17225</v>
       </c>
@@ -8939,7 +8948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" s="1">
         <v>17226</v>
       </c>
@@ -8959,7 +8968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" s="1">
         <v>17227</v>
       </c>
@@ -8979,7 +8988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" s="1">
         <v>17228</v>
       </c>
@@ -8999,7 +9008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" s="1">
         <v>17229</v>
       </c>
@@ -9013,7 +9022,7 @@
         <v>122</v>
       </c>
       <c r="H333" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I333" t="s">
         <v>36</v>

</xml_diff>